<commit_message>
included files for Li
</commit_message>
<xml_diff>
--- a/config/becExpConfig/parameterUnit.csv.xlsx
+++ b/config/becExpConfig/parameterUnit.csv.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoc\Documents\MMUser\config\becExpConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\_Li\Machine Code\MuscleMuseum\.config\becExpConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E773D7-F5FF-4BC2-A747-95181897BBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A8B451-AA35-4580-A6B7-E6BB2E848554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26970" yWindow="705" windowWidth="25695" windowHeight="14190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +25,208 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
+  <si>
+    <t>cMOT_tot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curveField2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1PumpTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>divisor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dummy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dummy2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>evapStageA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>evapStageD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeshbachField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeshbachField2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GMtime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCOGM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HFIMCDetuning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hfsnapdowntime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HFSnapTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMCDetuning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMCNonInter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IterationNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KPRampTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KP1VVA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KP2VVA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOTcDPvcoV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOT_load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M1Picomotor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>steps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mtramptime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ODT1PID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ODT2PID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ODTrampspeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpticalEvap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>randomRealization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relayTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>repump_flash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>speedscale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tau</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tdktime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TDKMOTV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>TOF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>XFHTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XV_max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XV_NI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>\mu s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -49,24 +245,240 @@
     <t>CiceroLogTime</t>
   </si>
   <si>
+    <t>ODTHoldTime</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>ODThold</t>
+  </si>
+  <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>latticehold</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>xvlattice</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>ZS_NI</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>xvramptime</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>xvPiPulse</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>plugvva</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>MuHold</t>
+  </si>
+  <si>
+    <t>NIRampTime</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>partialevaptime</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>curveField</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>hw_xvlattice</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>hw_XvLattice</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>hw_PdModDepth</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>hw_PdModPhase</t>
+  </si>
+  <si>
+    <t>Rad</t>
+  </si>
+  <si>
+    <t>PTENMOTV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>MTramptime</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>tdksnapon</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>MTsnapon</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>RFVVA</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>SXFTime</t>
+  </si>
+  <si>
+    <t>LatticeScope_CH1_Mean</t>
+  </si>
+  <si>
+    <t>dummy3</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>rampspeed</t>
+  </si>
+  <si>
+    <t>ms/V</t>
+  </si>
+  <si>
+    <t>sxfendpoint</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>sxfstartpoint</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>hw_RfKnife</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>hw_SXEndPoint</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>hw_SXStartPoint</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>NIhold</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>HfHoldTime</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>hw_SdCalibFreqStart</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>hw_SdRabiDepth</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>hw_XvNi</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>ZS_HF</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>vertfieldgrad</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>LatticeScope_Ch3_Mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -80,7 +492,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -88,15 +500,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -374,28 +788,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="true" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.73046875" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" customWidth="1"/>
-    <col min="3" max="4" width="12.265625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="true"/>
+    <col min="2" max="2" width="21.5703125" customWidth="true"/>
+    <col min="3" max="4" width="12.28515625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -403,18 +817,662 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+    <row r="6">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>85</v>
+      </c>
+      <c r="B66" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>99</v>
+      </c>
+      <c r="B73" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>103</v>
+      </c>
+      <c r="B75" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>105</v>
+      </c>
+      <c r="B76" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>107</v>
+      </c>
+      <c r="B77" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>109</v>
+      </c>
+      <c r="B78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>115</v>
+      </c>
+      <c r="B81" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B82" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>119</v>
+      </c>
+      <c r="B83" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B87" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>